<commit_message>
Version 2.4 # 2024-24-11
</commit_message>
<xml_diff>
--- a/results/Table1.xlsx
+++ b/results/Table1.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="91">
   <si>
     <t xml:space="preserve">Variable</t>
   </si>
@@ -182,18 +182,18 @@
     <t xml:space="preserve">Comorbidity (%)</t>
   </si>
   <si>
+    <t xml:space="preserve">Not Present</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   93 (51.7) </t>
+  </si>
+  <si>
     <t xml:space="preserve">Present</t>
   </si>
   <si>
     <t xml:space="preserve">   87 (48.3) </t>
   </si>
   <si>
-    <t xml:space="preserve">Not present</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   93 (51.7) </t>
-  </si>
-  <si>
     <t xml:space="preserve">Age at diagnosis (%)</t>
   </si>
   <si>
@@ -279,6 +279,12 @@
   </si>
   <si>
     <t xml:space="preserve">   31 (17.5) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Falls (%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  126 (70.0) </t>
   </si>
 </sst>
 </file>
@@ -1033,6 +1039,28 @@
         <v>88</v>
       </c>
     </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>89</v>
+      </c>
+      <c r="B39" t="s">
+        <v>77</v>
+      </c>
+      <c r="C39" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>4</v>
+      </c>
+      <c r="B40" t="s">
+        <v>79</v>
+      </c>
+      <c r="C40" t="s">
+        <v>49</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>

<commit_message>
newest versions of files
</commit_message>
<xml_diff>
--- a/results/Table1.xlsx
+++ b/results/Table1.xlsx
@@ -12,23 +12,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
     <t xml:space="preserve">Variable</t>
   </si>
   <si>
-    <t xml:space="preserve">level</t>
-  </si>
-  <si>
     <t xml:space="preserve">Overall</t>
   </si>
   <si>
     <t xml:space="preserve">n</t>
   </si>
   <si>
-    <t xml:space="preserve"/>
-  </si>
-  <si>
     <t xml:space="preserve">  181</t>
   </si>
   <si>
@@ -41,103 +35,64 @@
     <t xml:space="preserve">Age categorized (%)</t>
   </si>
   <si>
-    <t xml:space="preserve">≤ 60 years</t>
+    <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   ≤ 60 years</t>
   </si>
   <si>
     <t xml:space="preserve">   60 (33.3) </t>
   </si>
   <si>
-    <t xml:space="preserve">61 - 69 years</t>
+    <t xml:space="preserve">   61 - 69 years</t>
   </si>
   <si>
     <t xml:space="preserve">   58 (32.2) </t>
   </si>
   <si>
-    <t xml:space="preserve">≥ 70 years</t>
+    <t xml:space="preserve">   ≥ 70 years</t>
   </si>
   <si>
     <t xml:space="preserve">   62 (34.4) </t>
   </si>
   <si>
-    <t xml:space="preserve">Gender (%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Male</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   92 (50.8) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Female</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   88 (48.6) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Divers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    1 ( 0.6) </t>
+    <t xml:space="preserve">Gender = Female (%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   88 (48.9) </t>
   </si>
   <si>
     <t xml:space="preserve">Education level (%)</t>
   </si>
   <si>
-    <t xml:space="preserve">Primary school</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Higher secondary school</t>
+    <t xml:space="preserve">   Primary school</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Higher secondary school</t>
   </si>
   <si>
     <t xml:space="preserve">   46 (25.6) </t>
   </si>
   <si>
-    <t xml:space="preserve">University degree or higher</t>
+    <t xml:space="preserve">   University degree or higher</t>
   </si>
   <si>
     <t xml:space="preserve">   74 (41.1) </t>
   </si>
   <si>
-    <t xml:space="preserve">Financial stability (%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Most of the time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  171 (96.1) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Some of the time or less</t>
+    <t xml:space="preserve">Financial stability = Some of the time or less (%)</t>
   </si>
   <si>
     <t xml:space="preserve">    7 ( 3.9) </t>
   </si>
   <si>
-    <t xml:space="preserve">Family status (%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Without a partner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   44 (24.3) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">With a partner</t>
+    <t xml:space="preserve">Family status = With a partner (%)</t>
   </si>
   <si>
     <t xml:space="preserve">  137 (75.7) </t>
   </si>
   <si>
-    <t xml:space="preserve">Household situation (%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Independently</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  163 (90.1) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">With professional support</t>
+    <t xml:space="preserve">Household situation = With professional support (%)</t>
   </si>
   <si>
     <t xml:space="preserve">   18 ( 9.9) </t>
@@ -146,64 +101,31 @@
     <t xml:space="preserve">Living area (%)</t>
   </si>
   <si>
-    <t xml:space="preserve">Large city</t>
+    <t xml:space="preserve">   Large city</t>
   </si>
   <si>
     <t xml:space="preserve">   53 (29.4) </t>
   </si>
   <si>
-    <t xml:space="preserve">Medium-small city</t>
+    <t xml:space="preserve">   Medium-small city</t>
   </si>
   <si>
     <t xml:space="preserve">   73 (40.6) </t>
   </si>
   <si>
-    <t xml:space="preserve">Rural area</t>
+    <t xml:space="preserve">   Rural area</t>
   </si>
   <si>
     <t xml:space="preserve">   54 (30.0) </t>
   </si>
   <si>
-    <t xml:space="preserve">Depression (%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No depression</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   70 (40.7) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Impaired quality of life</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  102 (59.3) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Comorbidity (%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Not Present</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   93 (51.7) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Present</t>
+    <t xml:space="preserve">Comorbidity = Present (%)</t>
   </si>
   <si>
     <t xml:space="preserve">   87 (48.3) </t>
   </si>
   <si>
-    <t xml:space="preserve">Age at diagnosis (%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;50 years</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   48 (26.7) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">≥50 years</t>
+    <t xml:space="preserve">Age at diagnosis &lt;50 years = No (%)</t>
   </si>
   <si>
     <t xml:space="preserve">  132 (73.3) </t>
@@ -212,76 +134,55 @@
     <t xml:space="preserve">Time since diagnosis (%)</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;2 years</t>
+    <t xml:space="preserve">   &lt;2 years</t>
   </si>
   <si>
     <t xml:space="preserve">   29 (16.0) </t>
   </si>
   <si>
-    <t xml:space="preserve">2-5 years</t>
+    <t xml:space="preserve">   2-5 years</t>
   </si>
   <si>
     <t xml:space="preserve">   49 (27.1) </t>
   </si>
   <si>
-    <t xml:space="preserve">5-10 years</t>
+    <t xml:space="preserve">   5-10 years</t>
   </si>
   <si>
     <t xml:space="preserve">   47 (26.0) </t>
   </si>
   <si>
-    <t xml:space="preserve">10-15 years</t>
+    <t xml:space="preserve">   10-15 years</t>
   </si>
   <si>
     <t xml:space="preserve">   31 (17.1) </t>
   </si>
   <si>
-    <t xml:space="preserve">&gt;15 years</t>
+    <t xml:space="preserve">   &gt;15 years</t>
   </si>
   <si>
     <t xml:space="preserve">   25 (13.8) </t>
   </si>
   <si>
-    <t xml:space="preserve">Sleep disturbances (%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No</t>
+    <t xml:space="preserve">Sleep disturbances = No (%)</t>
   </si>
   <si>
     <t xml:space="preserve">   76 (42.0) </t>
   </si>
   <si>
-    <t xml:space="preserve">Yes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  105 (58.0) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Motor symptoms fluctuation (%)</t>
+    <t xml:space="preserve">Motor symptoms fluctuation = No (%)</t>
   </si>
   <si>
     <t xml:space="preserve">   52 (28.7) </t>
   </si>
   <si>
-    <t xml:space="preserve">  129 (71.3) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Assisted movement (%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No assisted movement</t>
+    <t xml:space="preserve">Assisted movement = No (%)</t>
   </si>
   <si>
     <t xml:space="preserve">  146 (82.5) </t>
   </si>
   <si>
-    <t xml:space="preserve">Assisted movement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   31 (17.5) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Falls (%)</t>
+    <t xml:space="preserve">Falls = No (%)</t>
   </si>
   <si>
     <t xml:space="preserve">  126 (70.0) </t>
@@ -616,9 +517,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
-    <col min="1" max="1" width="30.71" hidden="0" customWidth="1"/>
-    <col min="2" max="2" width="27.71" hidden="0" customWidth="1"/>
-    <col min="3" max="3" width="13.71" hidden="0" customWidth="1"/>
+    <col min="1" max="1" width="51.71" hidden="0" customWidth="1"/>
+    <col min="2" max="2" width="13.71" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -628,437 +528,245 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B13" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="B15" t="s">
-        <v>34</v>
-      </c>
-      <c r="C15" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
-      </c>
-      <c r="C16" t="s">
-        <v>37</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="B17" t="s">
-        <v>39</v>
-      </c>
-      <c r="C17" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="B18" t="s">
-        <v>41</v>
-      </c>
-      <c r="C18" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="B19" t="s">
-        <v>44</v>
-      </c>
-      <c r="C19" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>4</v>
+        <v>35</v>
       </c>
       <c r="B20" t="s">
-        <v>46</v>
-      </c>
-      <c r="C20" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>4</v>
+        <v>37</v>
       </c>
       <c r="B21" t="s">
-        <v>48</v>
-      </c>
-      <c r="C21" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="B22" t="s">
-        <v>51</v>
-      </c>
-      <c r="C22" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="B23" t="s">
-        <v>53</v>
-      </c>
-      <c r="C23" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="B24" t="s">
-        <v>56</v>
-      </c>
-      <c r="C24" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>4</v>
+        <v>44</v>
       </c>
       <c r="B25" t="s">
-        <v>58</v>
-      </c>
-      <c r="C25" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="B26" t="s">
-        <v>61</v>
-      </c>
-      <c r="C26" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>4</v>
+        <v>48</v>
       </c>
       <c r="B27" t="s">
-        <v>63</v>
-      </c>
-      <c r="C27" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="B28" t="s">
-        <v>66</v>
-      </c>
-      <c r="C28" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>4</v>
+        <v>52</v>
       </c>
       <c r="B29" t="s">
-        <v>68</v>
-      </c>
-      <c r="C29" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>4</v>
+        <v>54</v>
       </c>
       <c r="B30" t="s">
-        <v>70</v>
-      </c>
-      <c r="C30" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>4</v>
+        <v>56</v>
       </c>
       <c r="B31" t="s">
-        <v>72</v>
-      </c>
-      <c r="C31" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="s">
-        <v>4</v>
-      </c>
-      <c r="B32" t="s">
-        <v>74</v>
-      </c>
-      <c r="C32" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="s">
-        <v>76</v>
-      </c>
-      <c r="B33" t="s">
-        <v>77</v>
-      </c>
-      <c r="C33" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="s">
-        <v>4</v>
-      </c>
-      <c r="B34" t="s">
-        <v>79</v>
-      </c>
-      <c r="C34" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="s">
-        <v>81</v>
-      </c>
-      <c r="B35" t="s">
-        <v>77</v>
-      </c>
-      <c r="C35" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="s">
-        <v>4</v>
-      </c>
-      <c r="B36" t="s">
-        <v>79</v>
-      </c>
-      <c r="C36" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="s">
-        <v>84</v>
-      </c>
-      <c r="B37" t="s">
-        <v>85</v>
-      </c>
-      <c r="C37" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="s">
-        <v>4</v>
-      </c>
-      <c r="B38" t="s">
-        <v>87</v>
-      </c>
-      <c r="C38" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="s">
-        <v>89</v>
-      </c>
-      <c r="B39" t="s">
-        <v>77</v>
-      </c>
-      <c r="C39" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="s">
-        <v>4</v>
-      </c>
-      <c r="B40" t="s">
-        <v>79</v>
-      </c>
-      <c r="C40" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>